<commit_message>
Update the requirement documents
</commit_message>
<xml_diff>
--- a/Docs/forms fields.xlsx
+++ b/Docs/forms fields.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
   <si>
     <t>Personal Information</t>
   </si>
@@ -78,9 +78,6 @@
     <t>dropdown list</t>
   </si>
   <si>
-    <t>if the gender was male mility info form shows up</t>
-  </si>
-  <si>
     <t>military status</t>
   </si>
   <si>
@@ -150,21 +147,6 @@
     <t>dropdown list(Master - PhD)</t>
   </si>
   <si>
-    <t>Department 1</t>
-  </si>
-  <si>
-    <t>Department 1 topics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> multi select list</t>
-  </si>
-  <si>
-    <t>Department 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Department 2 topics </t>
-  </si>
-  <si>
     <t>If the applied degree was PhD The academic  background displays twic one for Bachelor info and one for the master info</t>
   </si>
   <si>
@@ -195,9 +177,6 @@
     <t>university</t>
   </si>
   <si>
-    <t>Master Info</t>
-  </si>
-  <si>
     <t>English Level Information</t>
   </si>
   <si>
@@ -228,9 +207,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Refrence</t>
-  </si>
-  <si>
     <t>Required 3 refrences</t>
   </si>
   <si>
@@ -295,13 +271,193 @@
   </si>
   <si>
     <t>datepicker</t>
+  </si>
+  <si>
+    <t>if the gender was male mility info become mandatory</t>
+  </si>
+  <si>
+    <t>Academic Interest Priority one</t>
+  </si>
+  <si>
+    <t>Drop down list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topics </t>
+  </si>
+  <si>
+    <t>Multi select dropdown list</t>
+  </si>
+  <si>
+    <t>Academic Interest Priority Two</t>
+  </si>
+  <si>
+    <t>Master Info (This form will be displayed in case of the applied degree was PhD)</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Required Files</t>
+  </si>
+  <si>
+    <t>Export data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button to export the applicant data to pdf </t>
+  </si>
+  <si>
+    <t>List of required files</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Personal Photograph</t>
+    </r>
+  </si>
+  <si>
+    <t>International TOEFL score from 500 , or Academic ILETS from 5.0</t>
+  </si>
+  <si>
+    <t>Three letters of recommendation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MSc Summary – English</t>
+    </r>
+  </si>
+  <si>
+    <t>BSc and MSc transcript(s)  - English *</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BSc and MSc certificate(s)  –  English *</t>
+    </r>
+  </si>
+  <si>
+    <t>Statement of purpose(Statement of your reasons for applying for E-JUST*</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application form signed(The exported PDF )*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Military Certificate</t>
+    </r>
+  </si>
+  <si>
+    <t>National ID card (Both sides) and Passport (If available).</t>
+  </si>
+  <si>
+    <t>Marriage Certificate (Both sides)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Children birth certificate</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +478,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -387,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +565,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,6 +574,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,16 +593,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,13 +896,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -827,14 +1002,14 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="13"/>
+      <c r="A15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -842,7 +1017,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -850,7 +1025,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
@@ -858,7 +1033,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
@@ -866,17 +1041,17 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -884,7 +1059,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
@@ -892,7 +1067,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>16</v>
@@ -900,7 +1075,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -908,7 +1083,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
@@ -916,7 +1091,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
@@ -924,7 +1099,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -932,24 +1107,24 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -957,7 +1132,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
@@ -965,7 +1140,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
@@ -973,40 +1148,40 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
+      <c r="A37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -1014,314 +1189,416 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="41" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="13"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B69" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="70" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="7"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" t="s">
         <v>57</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    </row>
+    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>58</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B72" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="73" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="7"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B68" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="6"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="6"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="7"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" t="s">
-        <v>66</v>
-      </c>
+      <c r="B74" s="10"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="15" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A46:E46"/>
+  <mergeCells count="16">
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="A72:E72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A44:E44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1346,108 +1623,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="A5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="A6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>80</v>
+      <c r="A9" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>81</v>
+      <c r="A10" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>82</v>
+      <c r="A11" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>83</v>
+      <c r="A12" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>